<commit_message>
Add rpm via CAN
rpm via CAN bus works
</commit_message>
<xml_diff>
--- a/STM32F469_TouchGFX_v2/TouchGFX/assets/texts/texts.xlsx
+++ b/STM32F469_TouchGFX_v2/TouchGFX/assets/texts/texts.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5997" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6327" uniqueCount="91">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -279,6 +279,24 @@
   </si>
   <si>
     <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
   </si>
 </sst>
 </file>
@@ -1785,7 +1803,7 @@
         <v>80</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="E4" t="s">
         <v>64</v>
@@ -1839,14 +1857,46 @@
         <v>43</v>
       </c>
       <c r="E7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="2:10"/>
-    <row r="9" spans="2:10"/>
+    <row r="8" spans="2:10">
+      <c r="B8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="B9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" t="s">
+        <v>90</v>
+      </c>
+      <c r="F9" t="s">
+        <v>44</v>
+      </c>
+    </row>
     <row r="10"/>
     <row r="11"/>
   </sheetData>

</xml_diff>

<commit_message>
Replace texts with icons
Icons for pFuel, tWat, tOil and pOil added instead of texts
</commit_message>
<xml_diff>
--- a/STM32F469_TouchGFX_v2/TouchGFX/assets/texts/texts.xlsx
+++ b/STM32F469_TouchGFX_v2/TouchGFX/assets/texts/texts.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19983" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20571" uniqueCount="229">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -807,6 +807,9 @@
   </si>
   <si>
     <t xml:space="preserve">consola.ttf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9</t>
   </si>
 </sst>
 </file>
@@ -2347,7 +2350,7 @@
         <v>80</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="E6" t="s">
         <v>64</v>
@@ -2367,7 +2370,7 @@
         <v>43</v>
       </c>
       <c r="E7" t="s">
-        <v>85</v>
+        <v>228</v>
       </c>
       <c r="F7" t="s">
         <v>44</v>
@@ -2494,72 +2497,24 @@
     </row>
     <row r="15">
       <c r="B15" t="s">
-        <v>97</v>
+        <v>222</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>80</v>
       </c>
       <c r="D15" t="s">
         <v>43</v>
       </c>
       <c r="E15" t="s">
-        <v>99</v>
+        <v>223</v>
       </c>
       <c r="F15" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16">
-      <c r="B16" t="s">
-        <v>107</v>
-      </c>
-      <c r="C16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" t="s">
-        <v>119</v>
-      </c>
-      <c r="F16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="B17" t="s">
-        <v>112</v>
-      </c>
-      <c r="C17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" t="s">
-        <v>86</v>
-      </c>
-      <c r="E17" t="s">
-        <v>151</v>
-      </c>
-      <c r="F17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="B18" t="s">
-        <v>222</v>
-      </c>
-      <c r="C18" t="s">
-        <v>80</v>
-      </c>
-      <c r="D18" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" t="s">
-        <v>223</v>
-      </c>
-      <c r="F18" t="s">
-        <v>44</v>
-      </c>
-    </row>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18"/>
   </sheetData>
   <sheetProtection sheet="0" objects="0" scenarios="0" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Add button for clutch
PA1 and PGA 12 are used for the button. Clutch opens/closes once per actuation.
Add function clutch()
</commit_message>
<xml_diff>
--- a/STM32F469_TouchGFX_v2/TouchGFX/assets/texts/texts.xlsx
+++ b/STM32F469_TouchGFX_v2/TouchGFX/assets/texts/texts.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20571" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24992" uniqueCount="253">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -810,6 +810,78 @@
   </si>
   <si>
     <t xml:space="preserve">9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coure.ttf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cour.ttf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typography_01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rpm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">km</t>
+  </si>
+  <si>
+    <t xml:space="preserve">km/h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">°</t>
+  </si>
+  <si>
+    <t xml:space="preserve">°C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gear</t>
   </si>
 </sst>
 </file>
@@ -2035,7 +2107,7 @@
         <v>35</v>
       </c>
       <c r="D4">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -2170,6 +2242,28 @@
       </c>
     </row>
     <row r="8" spans="2:15">
+      <c r="B8" t="s">
+        <v>236</v>
+      </c>
+      <c r="C8" t="s">
+        <v>227</v>
+      </c>
+      <c r="D8">
+        <v>150</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" t="s">
+        <v>217</v>
+      </c>
+      <c r="H8" t="s">
+        <v>217</v>
+      </c>
+      <c r="I8"/>
       <c r="K8" s="7" t="s">
         <v>10</v>
       </c>
@@ -2313,7 +2407,7 @@
         <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>80</v>
+        <v>236</v>
       </c>
       <c r="D4" t="s">
         <v>86</v>
@@ -2330,7 +2424,7 @@
         <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>80</v>
+        <v>236</v>
       </c>
       <c r="D5" t="s">
         <v>43</v>
@@ -2347,7 +2441,7 @@
         <v>70</v>
       </c>
       <c r="C6" t="s">
-        <v>80</v>
+        <v>236</v>
       </c>
       <c r="D6" t="s">
         <v>86</v>
@@ -2364,7 +2458,7 @@
         <v>82</v>
       </c>
       <c r="C7" t="s">
-        <v>80</v>
+        <v>236</v>
       </c>
       <c r="D7" t="s">
         <v>43</v>
@@ -2378,7 +2472,7 @@
     </row>
     <row r="8" spans="2:10">
       <c r="B8" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C8" t="s">
         <v>80</v>
@@ -2395,16 +2489,16 @@
     </row>
     <row r="9" spans="2:10">
       <c r="B9" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C9" t="s">
         <v>80</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="E9" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="F9" t="s">
         <v>44</v>
@@ -2412,16 +2506,16 @@
     </row>
     <row r="10">
       <c r="B10" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C10" t="s">
         <v>80</v>
       </c>
       <c r="D10" t="s">
-        <v>86</v>
+        <v>43</v>
       </c>
       <c r="E10" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
       <c r="F10" t="s">
         <v>44</v>
@@ -2429,7 +2523,7 @@
     </row>
     <row r="11">
       <c r="B11" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C11" t="s">
         <v>80</v>
@@ -2446,7 +2540,7 @@
     </row>
     <row r="12">
       <c r="B12" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C12" t="s">
         <v>80</v>
@@ -2463,16 +2557,16 @@
     </row>
     <row r="13">
       <c r="B13" t="s">
-        <v>95</v>
+        <v>222</v>
       </c>
       <c r="C13" t="s">
         <v>80</v>
       </c>
       <c r="D13" t="s">
-        <v>86</v>
+        <v>43</v>
       </c>
       <c r="E13" t="s">
-        <v>64</v>
+        <v>223</v>
       </c>
       <c r="F13" t="s">
         <v>44</v>
@@ -2480,16 +2574,16 @@
     </row>
     <row r="14">
       <c r="B14" t="s">
-        <v>96</v>
+        <v>231</v>
       </c>
       <c r="C14" t="s">
-        <v>80</v>
+        <v>236</v>
       </c>
       <c r="D14" t="s">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="E14" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="F14" t="s">
         <v>44</v>
@@ -2497,24 +2591,174 @@
     </row>
     <row r="15">
       <c r="B15" t="s">
-        <v>222</v>
+        <v>232</v>
       </c>
       <c r="C15" t="s">
-        <v>80</v>
+        <v>236</v>
       </c>
       <c r="D15" t="s">
         <v>43</v>
       </c>
       <c r="E15" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="F15" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16"/>
-    <row r="17"/>
-    <row r="18"/>
+    <row r="16">
+      <c r="B16" t="s">
+        <v>234</v>
+      </c>
+      <c r="C16" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="s">
+        <v>235</v>
+      </c>
+      <c r="C17" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" t="s">
+        <v>223</v>
+      </c>
+      <c r="F17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="s">
+        <v>237</v>
+      </c>
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" t="s">
+        <v>238</v>
+      </c>
+      <c r="F18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="s">
+        <v>239</v>
+      </c>
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" t="s">
+        <v>241</v>
+      </c>
+      <c r="F19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="s">
+        <v>242</v>
+      </c>
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" t="s">
+        <v>244</v>
+      </c>
+      <c r="F20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="s">
+        <v>245</v>
+      </c>
+      <c r="C21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" t="s">
+        <v>244</v>
+      </c>
+      <c r="F21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="s">
+        <v>246</v>
+      </c>
+      <c r="C22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" t="s">
+        <v>248</v>
+      </c>
+      <c r="F22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="s">
+        <v>249</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" t="s">
+        <v>248</v>
+      </c>
+      <c r="F23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="s">
+        <v>250</v>
+      </c>
+      <c r="C24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" t="s">
+        <v>252</v>
+      </c>
+      <c r="F24" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="0" objects="0" scenarios="0" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <mergeCells count="1">

</xml_diff>